<commit_message>
maj notes, planning, pluginjQ et README
</commit_message>
<xml_diff>
--- a/PlaningProjet.xlsx
+++ b/PlaningProjet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliemaieron/Documents/Formation/ChallengeColl/JJVL_wysiwyg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliemaieron/Documents/Formation/ChallengeColl/Project_wysiwyg_jjvl/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="440" windowWidth="20740" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Action</t>
   </si>
@@ -50,15 +50,6 @@
     <t>recherche solution git</t>
   </si>
   <si>
-    <t>Chercher le color picker</t>
-  </si>
-  <si>
-    <t>Chercher comment on crée un plugin Jquery</t>
-  </si>
-  <si>
-    <t>Planning de gestion de projet : EASYWYG</t>
-  </si>
-  <si>
     <t>initier la maquette HTML</t>
   </si>
   <si>
@@ -77,20 +68,78 @@
     <t>poursuite de la recherche sur la partie sélection et la partie saisie transformée</t>
   </si>
   <si>
-    <t>implémenter</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recherche SaSS  et gulp+ install </t>
   </si>
   <si>
     <t>install gul et saas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insertion des icons dans le HTMl </t>
+  </si>
+  <si>
+    <t>Début de mise en forme SCSS</t>
+  </si>
+  <si>
+    <t>Chercher et tester le color picker</t>
+  </si>
+  <si>
+    <t>Mise au propre des notes, planing</t>
+  </si>
+  <si>
+    <t>Draft du README</t>
+  </si>
+  <si>
+    <t>recherche sur Création de plugin Jquery</t>
+  </si>
+  <si>
+    <t>Intégration Color picker</t>
+  </si>
+  <si>
+    <t>Intégration contentEditable</t>
+  </si>
+  <si>
+    <t>Gestion dynamique de chaque élément</t>
+  </si>
+  <si>
+    <t>Finaliser le design css</t>
+  </si>
+  <si>
+    <t>filaniser le README</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Planning de gestion de projet : EASYWYG </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>js : encapsuler la selection et lui donner une fonction type (H1)</t>
+  </si>
+  <si>
+    <t>insertion id et class pour prépartion dynamisation dans le JS</t>
+  </si>
+  <si>
+    <t>rechercher des fonctionalité GetRange en JS</t>
+  </si>
+  <si>
+    <t>recherche de la modification d'un input pour le color picker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +149,13 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,7 +187,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="16"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -317,12 +381,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,15 +392,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -348,36 +403,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,261 +749,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="A1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="14" t="s">
+      <c r="H3" s="22"/>
+      <c r="I3" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="14">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="14">
+        <f ca="1">TODAY()</f>
+        <v>43280</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="14">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" ref="E6:E7" si="0">DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
+        <f ca="1">TODAY()</f>
+        <v>43280</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
+        <v>43279</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="14">
+        <f ca="1">TODAY()</f>
+        <v>43280</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="I7" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
         <f>DATE(2018,6,28)</f>
         <v>43279</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="14">
         <f>DATE(2018,6,28)</f>
         <v>43279</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="14">
+        <v>43280</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="14">
+        <f ca="1">TODAY()</f>
+        <v>43280</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5">
+      <c r="I8" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
         <f>DATE(2018,6,28)</f>
         <v>43279</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="B9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14">
+        <f>DATE(2018,6,28)</f>
+        <v>43279</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14">
         <f ca="1">TODAY()</f>
-        <v>43279</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <f>DATE(2018,6,28)</f>
-        <v>43279</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5">
-        <f>DATE(2018,6,28)</f>
-        <v>43279</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="5">
+        <v>43280</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
         <f ca="1">TODAY()</f>
-        <v>43279</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <f>DATE(2018,6,28)</f>
-        <v>43279</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="5">
+        <v>43280</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="14">
         <f ca="1">TODAY()</f>
-        <v>43279</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+        <v>43280</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="16"/>
     </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+    <row r="11" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="16"/>
     </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+    <row r="12" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+    <row r="13" spans="1:9" s="17" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rajout note de Linoel
</commit_message>
<xml_diff>
--- a/PlaningProjet.xlsx
+++ b/PlaningProjet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,12 +242,6 @@
       <b/>
       <sz val="20"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -435,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,13 +476,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -506,10 +500,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -791,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,7 +896,7 @@
       <c r="I5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
@@ -939,7 +930,7 @@
       <c r="I6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
@@ -973,7 +964,7 @@
       <c r="I7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -1005,7 +996,7 @@
       <c r="I8" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
@@ -1037,19 +1028,19 @@
       <c r="I9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <f ca="1">TODAY()</f>
-        <v>43282</v>
+        <v>43283</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="12">
         <f ca="1">TODAY()</f>
-        <v>43282</v>
+        <v>43283</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>27</v>
@@ -1069,19 +1060,19 @@
       <c r="I10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="18"/>
+      <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <f ca="1">TODAY()</f>
-        <v>43282</v>
+        <v>43283</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="12">
         <f ca="1">TODAY()</f>
-        <v>43282</v>
+        <v>43283</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>41</v>
@@ -1098,36 +1089,34 @@
       <c r="I11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="18"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <f ca="1">TODAY()</f>
+        <v>43283</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="12">
+        <f>DATE(2018,7,1)</f>
         <v>43282</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="12">
-        <f>DATE(2018,7,1)</f>
-        <v>43282</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="I12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="18"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:12" s="15" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <f ca="1">TODAY()</f>
-        <v>43282</v>
+        <v>43283</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -1141,7 +1130,7 @@
       <c r="I13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
@@ -1155,7 +1144,7 @@
       <c r="I14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
@@ -1169,7 +1158,7 @@
       <c r="I15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="18"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:12" s="4" customFormat="1" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -1183,7 +1172,7 @@
       <c r="I16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>